<commit_message>
ajout contrainte sur Task.status
status fixé à Completed 2e93db78070e4d33847090432f1d91b66ab60c14
</commit_message>
<xml_diff>
--- a/264-task-valeur-statut-à-vérifier/ig/all-profiles.xlsx
+++ b/264-task-valeur-statut-à-vérifier/ig/all-profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16664" uniqueCount="1250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16664" uniqueCount="1251">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-22T13:15:42+00:00</t>
+    <t>2024-11-22T13:30:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2851,6 +2851,9 @@
   </si>
   <si>
     <t>These states enable coordination of task status with off-the-shelf workflow solutions that support automation of tasks.</t>
+  </si>
+  <si>
+    <t>completed</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/task-status|4.0.1</t>
@@ -41849,7 +41852,7 @@
         <v>74</v>
       </c>
       <c r="T350" t="s" s="2">
-        <v>74</v>
+        <v>911</v>
       </c>
       <c r="U350" t="s" s="2">
         <v>74</v>
@@ -41870,7 +41873,7 @@
         <v>909</v>
       </c>
       <c r="AA350" t="s" s="2">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="AB350" t="s" s="2">
         <v>74</v>
@@ -41908,10 +41911,10 @@
         <v>858</v>
       </c>
       <c r="B351" t="s" s="2">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C351" t="s" s="2">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="D351" s="2"/>
       <c r="E351" t="s" s="2">
@@ -41937,13 +41940,13 @@
         <v>354</v>
       </c>
       <c r="M351" t="s" s="2">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="N351" t="s" s="2">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="O351" t="s" s="2">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="P351" s="2"/>
       <c r="Q351" t="s" s="2">
@@ -41972,7 +41975,7 @@
         <v>315</v>
       </c>
       <c r="Z351" t="s" s="2">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="AA351" t="s" s="2">
         <v>74</v>
@@ -41993,7 +41996,7 @@
         <v>74</v>
       </c>
       <c r="AG351" t="s" s="2">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="AH351" t="s" s="2">
         <v>75</v>
@@ -42013,10 +42016,10 @@
         <v>858</v>
       </c>
       <c r="B352" t="s" s="2">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C352" t="s" s="2">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="D352" s="2"/>
       <c r="E352" t="s" s="2">
@@ -42042,16 +42045,16 @@
         <v>354</v>
       </c>
       <c r="M352" t="s" s="2">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="N352" t="s" s="2">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="O352" t="s" s="2">
         <v>357</v>
       </c>
       <c r="P352" t="s" s="2">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="Q352" t="s" s="2">
         <v>74</v>
@@ -42079,7 +42082,7 @@
         <v>315</v>
       </c>
       <c r="Z352" t="s" s="2">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="AA352" t="s" s="2">
         <v>74</v>
@@ -42100,7 +42103,7 @@
         <v>74</v>
       </c>
       <c r="AG352" t="s" s="2">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="AH352" t="s" s="2">
         <v>75</v>
@@ -42120,10 +42123,10 @@
         <v>858</v>
       </c>
       <c r="B353" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C353" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="D353" s="2"/>
       <c r="E353" t="s" s="2">
@@ -42149,13 +42152,13 @@
         <v>103</v>
       </c>
       <c r="M353" t="s" s="2">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="N353" t="s" s="2">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="O353" t="s" s="2">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="P353" s="2"/>
       <c r="Q353" t="s" s="2">
@@ -42166,7 +42169,7 @@
         <v>74</v>
       </c>
       <c r="T353" t="s" s="2">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="U353" t="s" s="2">
         <v>74</v>
@@ -42184,10 +42187,10 @@
         <v>121</v>
       </c>
       <c r="Z353" t="s" s="2">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="AA353" t="s" s="2">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="AB353" t="s" s="2">
         <v>74</v>
@@ -42205,7 +42208,7 @@
         <v>74</v>
       </c>
       <c r="AG353" t="s" s="2">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="AH353" t="s" s="2">
         <v>82</v>
@@ -42225,10 +42228,10 @@
         <v>858</v>
       </c>
       <c r="B354" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C354" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="D354" s="2"/>
       <c r="E354" t="s" s="2">
@@ -42254,22 +42257,22 @@
         <v>103</v>
       </c>
       <c r="M354" t="s" s="2">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="N354" t="s" s="2">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="O354" t="s" s="2">
         <v>165</v>
       </c>
       <c r="P354" t="s" s="2">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="Q354" t="s" s="2">
         <v>74</v>
       </c>
       <c r="R354" t="s" s="2">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="S354" t="s" s="2">
         <v>74</v>
@@ -42293,10 +42296,10 @@
         <v>121</v>
       </c>
       <c r="Z354" t="s" s="2">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="AA354" t="s" s="2">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="AB354" t="s" s="2">
         <v>74</v>
@@ -42314,7 +42317,7 @@
         <v>74</v>
       </c>
       <c r="AG354" t="s" s="2">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="AH354" t="s" s="2">
         <v>75</v>
@@ -42334,10 +42337,10 @@
         <v>858</v>
       </c>
       <c r="B355" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C355" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="D355" s="2"/>
       <c r="E355" t="s" s="2">
@@ -42363,13 +42366,13 @@
         <v>354</v>
       </c>
       <c r="M355" t="s" s="2">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="N355" t="s" s="2">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="O355" t="s" s="2">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="P355" s="2"/>
       <c r="Q355" t="s" s="2">
@@ -42398,10 +42401,10 @@
         <v>315</v>
       </c>
       <c r="Z355" t="s" s="2">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="AA355" t="s" s="2">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="AB355" t="s" s="2">
         <v>74</v>
@@ -42419,7 +42422,7 @@
         <v>74</v>
       </c>
       <c r="AG355" t="s" s="2">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="AH355" t="s" s="2">
         <v>75</v>
@@ -42439,10 +42442,10 @@
         <v>858</v>
       </c>
       <c r="B356" t="s" s="2">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="C356" t="s" s="2">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="D356" s="2"/>
       <c r="E356" t="s" s="2">
@@ -42468,10 +42471,10 @@
         <v>141</v>
       </c>
       <c r="M356" t="s" s="2">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="N356" t="s" s="2">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="O356" t="s" s="2">
         <v>165</v>
@@ -42524,7 +42527,7 @@
         <v>74</v>
       </c>
       <c r="AG356" t="s" s="2">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="AH356" t="s" s="2">
         <v>75</v>
@@ -42544,10 +42547,10 @@
         <v>858</v>
       </c>
       <c r="B357" t="s" s="2">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C357" t="s" s="2">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="D357" s="2"/>
       <c r="E357" t="s" s="2">
@@ -42573,16 +42576,16 @@
         <v>838</v>
       </c>
       <c r="M357" t="s" s="2">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="N357" t="s" s="2">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="O357" t="s" s="2">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="P357" t="s" s="2">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="Q357" t="s" s="2">
         <v>74</v>
@@ -42631,7 +42634,7 @@
         <v>74</v>
       </c>
       <c r="AG357" t="s" s="2">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="AH357" t="s" s="2">
         <v>75</v>
@@ -42651,14 +42654,14 @@
         <v>858</v>
       </c>
       <c r="B358" t="s" s="2">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C358" t="s" s="2">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="D358" s="2"/>
       <c r="E358" t="s" s="2">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="F358" s="2"/>
       <c r="G358" t="s" s="2">
@@ -42680,16 +42683,16 @@
         <v>838</v>
       </c>
       <c r="M358" t="s" s="2">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="N358" t="s" s="2">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="O358" t="s" s="2">
         <v>389</v>
       </c>
       <c r="P358" t="s" s="2">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="Q358" t="s" s="2">
         <v>74</v>
@@ -42738,7 +42741,7 @@
         <v>74</v>
       </c>
       <c r="AG358" t="s" s="2">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="AH358" t="s" s="2">
         <v>75</v>
@@ -42758,10 +42761,10 @@
         <v>858</v>
       </c>
       <c r="B359" t="s" s="2">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C359" t="s" s="2">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="D359" s="2"/>
       <c r="E359" t="s" s="2">
@@ -42784,19 +42787,19 @@
         <v>83</v>
       </c>
       <c r="L359" t="s" s="2">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="M359" t="s" s="2">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="N359" t="s" s="2">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="O359" t="s" s="2">
         <v>389</v>
       </c>
       <c r="P359" t="s" s="2">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="Q359" t="s" s="2">
         <v>74</v>
@@ -42845,7 +42848,7 @@
         <v>74</v>
       </c>
       <c r="AG359" t="s" s="2">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="AH359" t="s" s="2">
         <v>75</v>
@@ -42865,10 +42868,10 @@
         <v>858</v>
       </c>
       <c r="B360" t="s" s="2">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C360" t="s" s="2">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="D360" s="2"/>
       <c r="E360" t="s" s="2">
@@ -42894,10 +42897,10 @@
         <v>444</v>
       </c>
       <c r="M360" t="s" s="2">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="N360" t="s" s="2">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="O360" t="s" s="2">
         <v>447</v>
@@ -42950,7 +42953,7 @@
         <v>74</v>
       </c>
       <c r="AG360" t="s" s="2">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="AH360" t="s" s="2">
         <v>75</v>
@@ -42970,14 +42973,14 @@
         <v>858</v>
       </c>
       <c r="B361" t="s" s="2">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C361" t="s" s="2">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D361" s="2"/>
       <c r="E361" t="s" s="2">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="F361" s="2"/>
       <c r="G361" t="s" s="2">
@@ -42999,14 +43002,14 @@
         <v>374</v>
       </c>
       <c r="M361" t="s" s="2">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="N361" t="s" s="2">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="O361" s="2"/>
       <c r="P361" t="s" s="2">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="Q361" t="s" s="2">
         <v>74</v>
@@ -43055,7 +43058,7 @@
         <v>74</v>
       </c>
       <c r="AG361" t="s" s="2">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="AH361" t="s" s="2">
         <v>75</v>
@@ -43064,7 +43067,7 @@
         <v>82</v>
       </c>
       <c r="AJ361" t="s" s="2">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="AK361" t="s" s="2">
         <v>95</v>
@@ -43075,14 +43078,14 @@
         <v>858</v>
       </c>
       <c r="B362" t="s" s="2">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C362" t="s" s="2">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D362" s="2"/>
       <c r="E362" t="s" s="2">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="F362" s="2"/>
       <c r="G362" t="s" s="2">
@@ -43104,14 +43107,14 @@
         <v>374</v>
       </c>
       <c r="M362" t="s" s="2">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="N362" t="s" s="2">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="O362" s="2"/>
       <c r="P362" t="s" s="2">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="Q362" t="s" s="2">
         <v>74</v>
@@ -43160,16 +43163,16 @@
         <v>74</v>
       </c>
       <c r="AG362" t="s" s="2">
+        <v>970</v>
+      </c>
+      <c r="AH362" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AI362" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AJ362" t="s" s="2">
         <v>969</v>
-      </c>
-      <c r="AH362" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AI362" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AJ362" t="s" s="2">
-        <v>968</v>
       </c>
       <c r="AK362" t="s" s="2">
         <v>95</v>
@@ -43180,10 +43183,10 @@
         <v>858</v>
       </c>
       <c r="B363" t="s" s="2">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C363" t="s" s="2">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D363" s="2"/>
       <c r="E363" t="s" s="2">
@@ -43206,19 +43209,19 @@
         <v>83</v>
       </c>
       <c r="L363" t="s" s="2">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="M363" t="s" s="2">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="N363" t="s" s="2">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="O363" t="s" s="2">
         <v>389</v>
       </c>
       <c r="P363" t="s" s="2">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="Q363" t="s" s="2">
         <v>74</v>
@@ -43267,7 +43270,7 @@
         <v>74</v>
       </c>
       <c r="AG363" t="s" s="2">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="AH363" t="s" s="2">
         <v>75</v>
@@ -43287,10 +43290,10 @@
         <v>858</v>
       </c>
       <c r="B364" t="s" s="2">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C364" t="s" s="2">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="D364" s="2"/>
       <c r="E364" t="s" s="2">
@@ -43316,16 +43319,16 @@
         <v>354</v>
       </c>
       <c r="M364" t="s" s="2">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="N364" t="s" s="2">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="O364" t="s" s="2">
         <v>357</v>
       </c>
       <c r="P364" t="s" s="2">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="Q364" t="s" s="2">
         <v>74</v>
@@ -43353,10 +43356,10 @@
         <v>107</v>
       </c>
       <c r="Z364" t="s" s="2">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="AA364" t="s" s="2">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="AB364" t="s" s="2">
         <v>74</v>
@@ -43374,7 +43377,7 @@
         <v>74</v>
       </c>
       <c r="AG364" t="s" s="2">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="AH364" t="s" s="2">
         <v>75</v>
@@ -43394,14 +43397,14 @@
         <v>858</v>
       </c>
       <c r="B365" t="s" s="2">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="C365" t="s" s="2">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="D365" s="2"/>
       <c r="E365" t="s" s="2">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F365" s="2"/>
       <c r="G365" t="s" s="2">
@@ -43420,19 +43423,19 @@
         <v>83</v>
       </c>
       <c r="L365" t="s" s="2">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="M365" t="s" s="2">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="N365" t="s" s="2">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="O365" t="s" s="2">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="P365" t="s" s="2">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="Q365" t="s" s="2">
         <v>74</v>
@@ -43481,7 +43484,7 @@
         <v>74</v>
       </c>
       <c r="AG365" t="s" s="2">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="AH365" t="s" s="2">
         <v>75</v>
@@ -43501,10 +43504,10 @@
         <v>858</v>
       </c>
       <c r="B366" t="s" s="2">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C366" t="s" s="2">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="D366" s="2"/>
       <c r="E366" t="s" s="2">
@@ -43527,19 +43530,19 @@
         <v>83</v>
       </c>
       <c r="L366" t="s" s="2">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="M366" t="s" s="2">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="N366" t="s" s="2">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="O366" t="s" s="2">
         <v>389</v>
       </c>
       <c r="P366" t="s" s="2">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="Q366" t="s" s="2">
         <v>74</v>
@@ -43588,7 +43591,7 @@
         <v>74</v>
       </c>
       <c r="AG366" t="s" s="2">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="AH366" t="s" s="2">
         <v>75</v>
@@ -43608,10 +43611,10 @@
         <v>858</v>
       </c>
       <c r="B367" t="s" s="2">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C367" t="s" s="2">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="D367" s="2"/>
       <c r="E367" t="s" s="2">
@@ -43637,13 +43640,13 @@
         <v>354</v>
       </c>
       <c r="M367" t="s" s="2">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="N367" t="s" s="2">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="O367" t="s" s="2">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="P367" s="2"/>
       <c r="Q367" t="s" s="2">
@@ -43672,7 +43675,7 @@
         <v>315</v>
       </c>
       <c r="Z367" t="s" s="2">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="AA367" t="s" s="2">
         <v>74</v>
@@ -43693,7 +43696,7 @@
         <v>74</v>
       </c>
       <c r="AG367" t="s" s="2">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="AH367" t="s" s="2">
         <v>75</v>
@@ -43713,10 +43716,10 @@
         <v>858</v>
       </c>
       <c r="B368" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="C368" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="D368" s="2"/>
       <c r="E368" t="s" s="2">
@@ -43742,13 +43745,13 @@
         <v>838</v>
       </c>
       <c r="M368" t="s" s="2">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="N368" t="s" s="2">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="O368" t="s" s="2">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="P368" s="2"/>
       <c r="Q368" t="s" s="2">
@@ -43798,7 +43801,7 @@
         <v>74</v>
       </c>
       <c r="AG368" t="s" s="2">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="AH368" t="s" s="2">
         <v>75</v>
@@ -43818,10 +43821,10 @@
         <v>858</v>
       </c>
       <c r="B369" t="s" s="2">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C369" t="s" s="2">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="D369" s="2"/>
       <c r="E369" t="s" s="2">
@@ -43844,13 +43847,13 @@
         <v>74</v>
       </c>
       <c r="L369" t="s" s="2">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="M369" t="s" s="2">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="N369" t="s" s="2">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="O369" t="s" s="2">
         <v>389</v>
@@ -43903,7 +43906,7 @@
         <v>74</v>
       </c>
       <c r="AG369" t="s" s="2">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="AH369" t="s" s="2">
         <v>75</v>
@@ -43923,10 +43926,10 @@
         <v>858</v>
       </c>
       <c r="B370" t="s" s="2">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C370" t="s" s="2">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="D370" s="2"/>
       <c r="E370" t="s" s="2">
@@ -43949,16 +43952,16 @@
         <v>74</v>
       </c>
       <c r="L370" t="s" s="2">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="M370" t="s" s="2">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="N370" t="s" s="2">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="O370" t="s" s="2">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="P370" s="2"/>
       <c r="Q370" t="s" s="2">
@@ -44008,7 +44011,7 @@
         <v>74</v>
       </c>
       <c r="AG370" t="s" s="2">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="AH370" t="s" s="2">
         <v>75</v>
@@ -44028,14 +44031,14 @@
         <v>858</v>
       </c>
       <c r="B371" t="s" s="2">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C371" t="s" s="2">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="D371" s="2"/>
       <c r="E371" t="s" s="2">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="F371" s="2"/>
       <c r="G371" t="s" s="2">
@@ -44054,16 +44057,16 @@
         <v>74</v>
       </c>
       <c r="L371" t="s" s="2">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="M371" t="s" s="2">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="N371" t="s" s="2">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="O371" t="s" s="2">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="P371" s="2"/>
       <c r="Q371" t="s" s="2">
@@ -44113,7 +44116,7 @@
         <v>74</v>
       </c>
       <c r="AG371" t="s" s="2">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="AH371" t="s" s="2">
         <v>75</v>
@@ -44133,10 +44136,10 @@
         <v>858</v>
       </c>
       <c r="B372" t="s" s="2">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="C372" t="s" s="2">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="D372" s="2"/>
       <c r="E372" t="s" s="2">
@@ -44162,14 +44165,14 @@
         <v>136</v>
       </c>
       <c r="M372" t="s" s="2">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="N372" t="s" s="2">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="O372" s="2"/>
       <c r="P372" t="s" s="2">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="Q372" t="s" s="2">
         <v>74</v>
@@ -44218,7 +44221,7 @@
         <v>74</v>
       </c>
       <c r="AG372" t="s" s="2">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="AH372" t="s" s="2">
         <v>75</v>
@@ -44238,10 +44241,10 @@
         <v>858</v>
       </c>
       <c r="B373" t="s" s="2">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C373" t="s" s="2">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="D373" s="2"/>
       <c r="E373" t="s" s="2">
@@ -44341,10 +44344,10 @@
         <v>858</v>
       </c>
       <c r="B374" t="s" s="2">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C374" t="s" s="2">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D374" s="2"/>
       <c r="E374" t="s" s="2">
@@ -44446,10 +44449,10 @@
         <v>858</v>
       </c>
       <c r="B375" t="s" s="2">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C375" t="s" s="2">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="D375" s="2"/>
       <c r="E375" t="s" s="2">
@@ -44553,10 +44556,10 @@
         <v>858</v>
       </c>
       <c r="B376" t="s" s="2">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C376" t="s" s="2">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="D376" s="2"/>
       <c r="E376" t="s" s="2">
@@ -44579,19 +44582,19 @@
         <v>74</v>
       </c>
       <c r="L376" t="s" s="2">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="M376" t="s" s="2">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="N376" t="s" s="2">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="O376" t="s" s="2">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="P376" t="s" s="2">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="Q376" t="s" s="2">
         <v>74</v>
@@ -44640,7 +44643,7 @@
         <v>74</v>
       </c>
       <c r="AG376" t="s" s="2">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="AH376" t="s" s="2">
         <v>75</v>
@@ -44660,10 +44663,10 @@
         <v>858</v>
       </c>
       <c r="B377" t="s" s="2">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C377" t="s" s="2">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="D377" s="2"/>
       <c r="E377" t="s" s="2">
@@ -44689,16 +44692,16 @@
         <v>444</v>
       </c>
       <c r="M377" t="s" s="2">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="N377" t="s" s="2">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="O377" t="s" s="2">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="P377" t="s" s="2">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="Q377" t="s" s="2">
         <v>74</v>
@@ -44747,7 +44750,7 @@
         <v>74</v>
       </c>
       <c r="AG377" t="s" s="2">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="AH377" t="s" s="2">
         <v>75</v>
@@ -44767,10 +44770,10 @@
         <v>858</v>
       </c>
       <c r="B378" t="s" s="2">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="C378" t="s" s="2">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="D378" s="2"/>
       <c r="E378" t="s" s="2">
@@ -44793,13 +44796,13 @@
         <v>74</v>
       </c>
       <c r="L378" t="s" s="2">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="M378" t="s" s="2">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="N378" t="s" s="2">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="O378" t="s" s="2">
         <v>389</v>
@@ -44852,7 +44855,7 @@
         <v>74</v>
       </c>
       <c r="AG378" t="s" s="2">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="AH378" t="s" s="2">
         <v>75</v>
@@ -44872,18 +44875,18 @@
         <v>858</v>
       </c>
       <c r="B379" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="C379" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D379" s="2"/>
       <c r="E379" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F379" s="2"/>
       <c r="G379" t="s" s="2">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="H379" t="s" s="2">
         <v>76</v>
@@ -44901,14 +44904,14 @@
         <v>136</v>
       </c>
       <c r="M379" t="s" s="2">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="N379" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O379" s="2"/>
       <c r="P379" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q379" t="s" s="2">
         <v>74</v>
@@ -44945,7 +44948,7 @@
         <v>74</v>
       </c>
       <c r="AC379" t="s" s="2">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="AD379" s="2"/>
       <c r="AE379" t="s" s="2">
@@ -44955,7 +44958,7 @@
         <v>153</v>
       </c>
       <c r="AG379" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH379" t="s" s="2">
         <v>75</v>
@@ -44975,10 +44978,10 @@
         <v>858</v>
       </c>
       <c r="B380" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C380" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D380" s="2"/>
       <c r="E380" t="s" s="2">
@@ -45078,10 +45081,10 @@
         <v>858</v>
       </c>
       <c r="B381" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="C381" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D381" s="2"/>
       <c r="E381" t="s" s="2">
@@ -45183,10 +45186,10 @@
         <v>858</v>
       </c>
       <c r="B382" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C382" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D382" s="2"/>
       <c r="E382" t="s" s="2">
@@ -45290,14 +45293,14 @@
         <v>858</v>
       </c>
       <c r="B383" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="C383" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D383" s="2"/>
       <c r="E383" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F383" s="2"/>
       <c r="G383" t="s" s="2">
@@ -45319,16 +45322,16 @@
         <v>354</v>
       </c>
       <c r="M383" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N383" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O383" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P383" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q383" t="s" s="2">
         <v>74</v>
@@ -45356,7 +45359,7 @@
         <v>315</v>
       </c>
       <c r="Z383" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA383" t="s" s="2">
         <v>74</v>
@@ -45377,7 +45380,7 @@
         <v>74</v>
       </c>
       <c r="AG383" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH383" t="s" s="2">
         <v>82</v>
@@ -45397,10 +45400,10 @@
         <v>858</v>
       </c>
       <c r="B384" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="C384" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D384" s="2"/>
       <c r="E384" t="s" s="2">
@@ -45423,13 +45426,13 @@
         <v>74</v>
       </c>
       <c r="L384" t="s" s="2">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="M384" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N384" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O384" s="2"/>
       <c r="P384" s="2"/>
@@ -45480,7 +45483,7 @@
         <v>74</v>
       </c>
       <c r="AG384" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH384" t="s" s="2">
         <v>82</v>
@@ -45500,16 +45503,16 @@
         <v>858</v>
       </c>
       <c r="B385" t="s" s="2">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C385" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D385" t="s" s="2">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="E385" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F385" s="2"/>
       <c r="G385" t="s" s="2">
@@ -45531,14 +45534,14 @@
         <v>136</v>
       </c>
       <c r="M385" t="s" s="2">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="N385" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O385" s="2"/>
       <c r="P385" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q385" t="s" s="2">
         <v>74</v>
@@ -45587,7 +45590,7 @@
         <v>74</v>
       </c>
       <c r="AG385" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH385" t="s" s="2">
         <v>75</v>
@@ -45607,10 +45610,10 @@
         <v>858</v>
       </c>
       <c r="B386" t="s" s="2">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C386" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D386" s="2"/>
       <c r="E386" t="s" s="2">
@@ -45710,10 +45713,10 @@
         <v>858</v>
       </c>
       <c r="B387" t="s" s="2">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="C387" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D387" s="2"/>
       <c r="E387" t="s" s="2">
@@ -45815,10 +45818,10 @@
         <v>858</v>
       </c>
       <c r="B388" t="s" s="2">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C388" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D388" s="2"/>
       <c r="E388" t="s" s="2">
@@ -45922,14 +45925,14 @@
         <v>858</v>
       </c>
       <c r="B389" t="s" s="2">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="C389" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D389" s="2"/>
       <c r="E389" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F389" s="2"/>
       <c r="G389" t="s" s="2">
@@ -45951,16 +45954,16 @@
         <v>354</v>
       </c>
       <c r="M389" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N389" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O389" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P389" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q389" t="s" s="2">
         <v>74</v>
@@ -45970,7 +45973,7 @@
         <v>74</v>
       </c>
       <c r="T389" t="s" s="2">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="U389" t="s" s="2">
         <v>74</v>
@@ -45988,7 +45991,7 @@
         <v>315</v>
       </c>
       <c r="Z389" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA389" t="s" s="2">
         <v>74</v>
@@ -46009,7 +46012,7 @@
         <v>74</v>
       </c>
       <c r="AG389" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH389" t="s" s="2">
         <v>82</v>
@@ -46029,10 +46032,10 @@
         <v>858</v>
       </c>
       <c r="B390" t="s" s="2">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="C390" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D390" s="2"/>
       <c r="E390" t="s" s="2">
@@ -46058,10 +46061,10 @@
         <v>112</v>
       </c>
       <c r="M390" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N390" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O390" s="2"/>
       <c r="P390" s="2"/>
@@ -46112,7 +46115,7 @@
         <v>74</v>
       </c>
       <c r="AG390" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH390" t="s" s="2">
         <v>82</v>
@@ -46132,16 +46135,16 @@
         <v>858</v>
       </c>
       <c r="B391" t="s" s="2">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C391" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D391" t="s" s="2">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E391" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F391" s="2"/>
       <c r="G391" t="s" s="2">
@@ -46163,14 +46166,14 @@
         <v>136</v>
       </c>
       <c r="M391" t="s" s="2">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="N391" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O391" s="2"/>
       <c r="P391" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q391" t="s" s="2">
         <v>74</v>
@@ -46219,7 +46222,7 @@
         <v>74</v>
       </c>
       <c r="AG391" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH391" t="s" s="2">
         <v>75</v>
@@ -46239,10 +46242,10 @@
         <v>858</v>
       </c>
       <c r="B392" t="s" s="2">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="C392" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D392" s="2"/>
       <c r="E392" t="s" s="2">
@@ -46342,10 +46345,10 @@
         <v>858</v>
       </c>
       <c r="B393" t="s" s="2">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C393" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D393" s="2"/>
       <c r="E393" t="s" s="2">
@@ -46447,10 +46450,10 @@
         <v>858</v>
       </c>
       <c r="B394" t="s" s="2">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="C394" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D394" s="2"/>
       <c r="E394" t="s" s="2">
@@ -46554,14 +46557,14 @@
         <v>858</v>
       </c>
       <c r="B395" t="s" s="2">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C395" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D395" s="2"/>
       <c r="E395" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F395" s="2"/>
       <c r="G395" t="s" s="2">
@@ -46583,16 +46586,16 @@
         <v>354</v>
       </c>
       <c r="M395" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N395" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O395" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P395" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q395" t="s" s="2">
         <v>74</v>
@@ -46602,7 +46605,7 @@
         <v>74</v>
       </c>
       <c r="T395" t="s" s="2">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="U395" t="s" s="2">
         <v>74</v>
@@ -46620,7 +46623,7 @@
         <v>315</v>
       </c>
       <c r="Z395" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA395" t="s" s="2">
         <v>74</v>
@@ -46641,7 +46644,7 @@
         <v>74</v>
       </c>
       <c r="AG395" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH395" t="s" s="2">
         <v>82</v>
@@ -46661,10 +46664,10 @@
         <v>858</v>
       </c>
       <c r="B396" t="s" s="2">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C396" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D396" s="2"/>
       <c r="E396" t="s" s="2">
@@ -46690,10 +46693,10 @@
         <v>141</v>
       </c>
       <c r="M396" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N396" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O396" s="2"/>
       <c r="P396" s="2"/>
@@ -46744,7 +46747,7 @@
         <v>74</v>
       </c>
       <c r="AG396" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH396" t="s" s="2">
         <v>82</v>
@@ -46764,16 +46767,16 @@
         <v>858</v>
       </c>
       <c r="B397" t="s" s="2">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="C397" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D397" t="s" s="2">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="E397" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F397" s="2"/>
       <c r="G397" t="s" s="2">
@@ -46795,14 +46798,14 @@
         <v>136</v>
       </c>
       <c r="M397" t="s" s="2">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="N397" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O397" s="2"/>
       <c r="P397" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q397" t="s" s="2">
         <v>74</v>
@@ -46851,7 +46854,7 @@
         <v>74</v>
       </c>
       <c r="AG397" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH397" t="s" s="2">
         <v>75</v>
@@ -46871,10 +46874,10 @@
         <v>858</v>
       </c>
       <c r="B398" t="s" s="2">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C398" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D398" s="2"/>
       <c r="E398" t="s" s="2">
@@ -46974,10 +46977,10 @@
         <v>858</v>
       </c>
       <c r="B399" t="s" s="2">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="C399" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D399" s="2"/>
       <c r="E399" t="s" s="2">
@@ -47079,10 +47082,10 @@
         <v>858</v>
       </c>
       <c r="B400" t="s" s="2">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C400" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D400" s="2"/>
       <c r="E400" t="s" s="2">
@@ -47186,14 +47189,14 @@
         <v>858</v>
       </c>
       <c r="B401" t="s" s="2">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="C401" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D401" s="2"/>
       <c r="E401" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F401" s="2"/>
       <c r="G401" t="s" s="2">
@@ -47215,16 +47218,16 @@
         <v>354</v>
       </c>
       <c r="M401" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N401" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O401" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P401" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q401" t="s" s="2">
         <v>74</v>
@@ -47234,7 +47237,7 @@
         <v>74</v>
       </c>
       <c r="T401" t="s" s="2">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="U401" t="s" s="2">
         <v>74</v>
@@ -47252,7 +47255,7 @@
         <v>315</v>
       </c>
       <c r="Z401" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA401" t="s" s="2">
         <v>74</v>
@@ -47273,7 +47276,7 @@
         <v>74</v>
       </c>
       <c r="AG401" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH401" t="s" s="2">
         <v>82</v>
@@ -47293,10 +47296,10 @@
         <v>858</v>
       </c>
       <c r="B402" t="s" s="2">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="C402" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D402" s="2"/>
       <c r="E402" t="s" s="2">
@@ -47322,10 +47325,10 @@
         <v>354</v>
       </c>
       <c r="M402" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N402" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O402" s="2"/>
       <c r="P402" s="2"/>
@@ -47356,7 +47359,7 @@
       </c>
       <c r="Z402" s="2"/>
       <c r="AA402" t="s" s="2">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="AB402" t="s" s="2">
         <v>74</v>
@@ -47374,7 +47377,7 @@
         <v>74</v>
       </c>
       <c r="AG402" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH402" t="s" s="2">
         <v>82</v>
@@ -47394,16 +47397,16 @@
         <v>858</v>
       </c>
       <c r="B403" t="s" s="2">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="C403" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D403" t="s" s="2">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="E403" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F403" s="2"/>
       <c r="G403" t="s" s="2">
@@ -47425,14 +47428,14 @@
         <v>136</v>
       </c>
       <c r="M403" t="s" s="2">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="N403" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O403" s="2"/>
       <c r="P403" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q403" t="s" s="2">
         <v>74</v>
@@ -47481,7 +47484,7 @@
         <v>74</v>
       </c>
       <c r="AG403" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH403" t="s" s="2">
         <v>75</v>
@@ -47501,10 +47504,10 @@
         <v>858</v>
       </c>
       <c r="B404" t="s" s="2">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="C404" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D404" s="2"/>
       <c r="E404" t="s" s="2">
@@ -47604,10 +47607,10 @@
         <v>858</v>
       </c>
       <c r="B405" t="s" s="2">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C405" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D405" s="2"/>
       <c r="E405" t="s" s="2">
@@ -47709,10 +47712,10 @@
         <v>858</v>
       </c>
       <c r="B406" t="s" s="2">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="C406" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D406" s="2"/>
       <c r="E406" t="s" s="2">
@@ -47816,14 +47819,14 @@
         <v>858</v>
       </c>
       <c r="B407" t="s" s="2">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C407" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D407" s="2"/>
       <c r="E407" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F407" s="2"/>
       <c r="G407" t="s" s="2">
@@ -47845,16 +47848,16 @@
         <v>354</v>
       </c>
       <c r="M407" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N407" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O407" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P407" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q407" t="s" s="2">
         <v>74</v>
@@ -47864,7 +47867,7 @@
         <v>74</v>
       </c>
       <c r="T407" t="s" s="2">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="U407" t="s" s="2">
         <v>74</v>
@@ -47882,7 +47885,7 @@
         <v>315</v>
       </c>
       <c r="Z407" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA407" t="s" s="2">
         <v>74</v>
@@ -47903,7 +47906,7 @@
         <v>74</v>
       </c>
       <c r="AG407" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH407" t="s" s="2">
         <v>82</v>
@@ -47923,10 +47926,10 @@
         <v>858</v>
       </c>
       <c r="B408" t="s" s="2">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C408" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D408" s="2"/>
       <c r="E408" t="s" s="2">
@@ -47952,10 +47955,10 @@
         <v>354</v>
       </c>
       <c r="M408" t="s" s="2">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="N408" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O408" s="2"/>
       <c r="P408" s="2"/>
@@ -47986,7 +47989,7 @@
       </c>
       <c r="Z408" s="2"/>
       <c r="AA408" t="s" s="2">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="AB408" t="s" s="2">
         <v>74</v>
@@ -48004,7 +48007,7 @@
         <v>74</v>
       </c>
       <c r="AG408" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH408" t="s" s="2">
         <v>82</v>
@@ -48024,16 +48027,16 @@
         <v>858</v>
       </c>
       <c r="B409" t="s" s="2">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="C409" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D409" t="s" s="2">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="E409" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F409" s="2"/>
       <c r="G409" t="s" s="2">
@@ -48055,14 +48058,14 @@
         <v>136</v>
       </c>
       <c r="M409" t="s" s="2">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="N409" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O409" s="2"/>
       <c r="P409" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q409" t="s" s="2">
         <v>74</v>
@@ -48111,7 +48114,7 @@
         <v>74</v>
       </c>
       <c r="AG409" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH409" t="s" s="2">
         <v>75</v>
@@ -48131,10 +48134,10 @@
         <v>858</v>
       </c>
       <c r="B410" t="s" s="2">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C410" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D410" s="2"/>
       <c r="E410" t="s" s="2">
@@ -48234,10 +48237,10 @@
         <v>858</v>
       </c>
       <c r="B411" t="s" s="2">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="C411" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D411" s="2"/>
       <c r="E411" t="s" s="2">
@@ -48339,10 +48342,10 @@
         <v>858</v>
       </c>
       <c r="B412" t="s" s="2">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C412" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D412" s="2"/>
       <c r="E412" t="s" s="2">
@@ -48446,14 +48449,14 @@
         <v>858</v>
       </c>
       <c r="B413" t="s" s="2">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="C413" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D413" s="2"/>
       <c r="E413" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F413" s="2"/>
       <c r="G413" t="s" s="2">
@@ -48475,16 +48478,16 @@
         <v>354</v>
       </c>
       <c r="M413" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N413" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O413" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P413" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q413" t="s" s="2">
         <v>74</v>
@@ -48494,7 +48497,7 @@
         <v>74</v>
       </c>
       <c r="T413" t="s" s="2">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="U413" t="s" s="2">
         <v>74</v>
@@ -48512,7 +48515,7 @@
         <v>315</v>
       </c>
       <c r="Z413" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA413" t="s" s="2">
         <v>74</v>
@@ -48533,7 +48536,7 @@
         <v>74</v>
       </c>
       <c r="AG413" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH413" t="s" s="2">
         <v>82</v>
@@ -48553,10 +48556,10 @@
         <v>858</v>
       </c>
       <c r="B414" t="s" s="2">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="C414" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D414" s="2"/>
       <c r="E414" t="s" s="2">
@@ -48579,13 +48582,13 @@
         <v>74</v>
       </c>
       <c r="L414" t="s" s="2">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="M414" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N414" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O414" s="2"/>
       <c r="P414" s="2"/>
@@ -48636,7 +48639,7 @@
         <v>74</v>
       </c>
       <c r="AG414" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH414" t="s" s="2">
         <v>82</v>
@@ -48656,16 +48659,16 @@
         <v>858</v>
       </c>
       <c r="B415" t="s" s="2">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="C415" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D415" t="s" s="2">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="E415" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F415" s="2"/>
       <c r="G415" t="s" s="2">
@@ -48687,14 +48690,14 @@
         <v>136</v>
       </c>
       <c r="M415" t="s" s="2">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="N415" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O415" s="2"/>
       <c r="P415" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q415" t="s" s="2">
         <v>74</v>
@@ -48743,7 +48746,7 @@
         <v>74</v>
       </c>
       <c r="AG415" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH415" t="s" s="2">
         <v>75</v>
@@ -48763,10 +48766,10 @@
         <v>858</v>
       </c>
       <c r="B416" t="s" s="2">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C416" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D416" s="2"/>
       <c r="E416" t="s" s="2">
@@ -48866,10 +48869,10 @@
         <v>858</v>
       </c>
       <c r="B417" t="s" s="2">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="C417" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D417" s="2"/>
       <c r="E417" t="s" s="2">
@@ -48971,10 +48974,10 @@
         <v>858</v>
       </c>
       <c r="B418" t="s" s="2">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C418" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D418" s="2"/>
       <c r="E418" t="s" s="2">
@@ -49078,14 +49081,14 @@
         <v>858</v>
       </c>
       <c r="B419" t="s" s="2">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="C419" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D419" s="2"/>
       <c r="E419" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F419" s="2"/>
       <c r="G419" t="s" s="2">
@@ -49107,16 +49110,16 @@
         <v>354</v>
       </c>
       <c r="M419" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N419" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O419" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P419" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q419" t="s" s="2">
         <v>74</v>
@@ -49126,7 +49129,7 @@
         <v>74</v>
       </c>
       <c r="T419" t="s" s="2">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="U419" t="s" s="2">
         <v>74</v>
@@ -49144,7 +49147,7 @@
         <v>315</v>
       </c>
       <c r="Z419" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA419" t="s" s="2">
         <v>74</v>
@@ -49165,7 +49168,7 @@
         <v>74</v>
       </c>
       <c r="AG419" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH419" t="s" s="2">
         <v>82</v>
@@ -49185,10 +49188,10 @@
         <v>858</v>
       </c>
       <c r="B420" t="s" s="2">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="C420" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D420" s="2"/>
       <c r="E420" t="s" s="2">
@@ -49214,10 +49217,10 @@
         <v>112</v>
       </c>
       <c r="M420" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N420" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O420" s="2"/>
       <c r="P420" s="2"/>
@@ -49268,7 +49271,7 @@
         <v>74</v>
       </c>
       <c r="AG420" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH420" t="s" s="2">
         <v>82</v>
@@ -49288,16 +49291,16 @@
         <v>858</v>
       </c>
       <c r="B421" t="s" s="2">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C421" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D421" t="s" s="2">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="E421" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F421" s="2"/>
       <c r="G421" t="s" s="2">
@@ -49319,14 +49322,14 @@
         <v>136</v>
       </c>
       <c r="M421" t="s" s="2">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="N421" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O421" s="2"/>
       <c r="P421" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q421" t="s" s="2">
         <v>74</v>
@@ -49375,7 +49378,7 @@
         <v>74</v>
       </c>
       <c r="AG421" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH421" t="s" s="2">
         <v>75</v>
@@ -49395,10 +49398,10 @@
         <v>858</v>
       </c>
       <c r="B422" t="s" s="2">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="C422" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D422" s="2"/>
       <c r="E422" t="s" s="2">
@@ -49498,10 +49501,10 @@
         <v>858</v>
       </c>
       <c r="B423" t="s" s="2">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="C423" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D423" s="2"/>
       <c r="E423" t="s" s="2">
@@ -49603,10 +49606,10 @@
         <v>858</v>
       </c>
       <c r="B424" t="s" s="2">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="C424" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D424" s="2"/>
       <c r="E424" t="s" s="2">
@@ -49710,14 +49713,14 @@
         <v>858</v>
       </c>
       <c r="B425" t="s" s="2">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="C425" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D425" s="2"/>
       <c r="E425" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F425" s="2"/>
       <c r="G425" t="s" s="2">
@@ -49739,16 +49742,16 @@
         <v>354</v>
       </c>
       <c r="M425" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N425" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O425" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P425" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q425" t="s" s="2">
         <v>74</v>
@@ -49758,7 +49761,7 @@
         <v>74</v>
       </c>
       <c r="T425" t="s" s="2">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="U425" t="s" s="2">
         <v>74</v>
@@ -49776,7 +49779,7 @@
         <v>315</v>
       </c>
       <c r="Z425" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA425" t="s" s="2">
         <v>74</v>
@@ -49797,7 +49800,7 @@
         <v>74</v>
       </c>
       <c r="AG425" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH425" t="s" s="2">
         <v>82</v>
@@ -49817,10 +49820,10 @@
         <v>858</v>
       </c>
       <c r="B426" t="s" s="2">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="C426" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D426" s="2"/>
       <c r="E426" t="s" s="2">
@@ -49846,10 +49849,10 @@
         <v>141</v>
       </c>
       <c r="M426" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N426" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O426" s="2"/>
       <c r="P426" s="2"/>
@@ -49900,7 +49903,7 @@
         <v>74</v>
       </c>
       <c r="AG426" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH426" t="s" s="2">
         <v>82</v>
@@ -49920,16 +49923,16 @@
         <v>858</v>
       </c>
       <c r="B427" t="s" s="2">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="C427" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D427" t="s" s="2">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="E427" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F427" s="2"/>
       <c r="G427" t="s" s="2">
@@ -49951,14 +49954,14 @@
         <v>136</v>
       </c>
       <c r="M427" t="s" s="2">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="N427" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O427" s="2"/>
       <c r="P427" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q427" t="s" s="2">
         <v>74</v>
@@ -50007,7 +50010,7 @@
         <v>74</v>
       </c>
       <c r="AG427" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH427" t="s" s="2">
         <v>75</v>
@@ -50027,10 +50030,10 @@
         <v>858</v>
       </c>
       <c r="B428" t="s" s="2">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C428" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D428" s="2"/>
       <c r="E428" t="s" s="2">
@@ -50130,10 +50133,10 @@
         <v>858</v>
       </c>
       <c r="B429" t="s" s="2">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="C429" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D429" s="2"/>
       <c r="E429" t="s" s="2">
@@ -50235,10 +50238,10 @@
         <v>858</v>
       </c>
       <c r="B430" t="s" s="2">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C430" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D430" s="2"/>
       <c r="E430" t="s" s="2">
@@ -50342,14 +50345,14 @@
         <v>858</v>
       </c>
       <c r="B431" t="s" s="2">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="C431" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D431" s="2"/>
       <c r="E431" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F431" s="2"/>
       <c r="G431" t="s" s="2">
@@ -50371,16 +50374,16 @@
         <v>354</v>
       </c>
       <c r="M431" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N431" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O431" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P431" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q431" t="s" s="2">
         <v>74</v>
@@ -50390,7 +50393,7 @@
         <v>74</v>
       </c>
       <c r="T431" t="s" s="2">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="U431" t="s" s="2">
         <v>74</v>
@@ -50408,7 +50411,7 @@
         <v>315</v>
       </c>
       <c r="Z431" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA431" t="s" s="2">
         <v>74</v>
@@ -50429,7 +50432,7 @@
         <v>74</v>
       </c>
       <c r="AG431" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH431" t="s" s="2">
         <v>82</v>
@@ -50449,10 +50452,10 @@
         <v>858</v>
       </c>
       <c r="B432" t="s" s="2">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="C432" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D432" s="2"/>
       <c r="E432" t="s" s="2">
@@ -50478,10 +50481,10 @@
         <v>354</v>
       </c>
       <c r="M432" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N432" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O432" s="2"/>
       <c r="P432" s="2"/>
@@ -50512,7 +50515,7 @@
       </c>
       <c r="Z432" s="2"/>
       <c r="AA432" t="s" s="2">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="AB432" t="s" s="2">
         <v>74</v>
@@ -50530,7 +50533,7 @@
         <v>74</v>
       </c>
       <c r="AG432" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH432" t="s" s="2">
         <v>82</v>
@@ -50550,16 +50553,16 @@
         <v>858</v>
       </c>
       <c r="B433" t="s" s="2">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="C433" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D433" t="s" s="2">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="E433" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F433" s="2"/>
       <c r="G433" t="s" s="2">
@@ -50581,14 +50584,14 @@
         <v>136</v>
       </c>
       <c r="M433" t="s" s="2">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="N433" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O433" s="2"/>
       <c r="P433" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q433" t="s" s="2">
         <v>74</v>
@@ -50637,7 +50640,7 @@
         <v>74</v>
       </c>
       <c r="AG433" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH433" t="s" s="2">
         <v>75</v>
@@ -50657,10 +50660,10 @@
         <v>858</v>
       </c>
       <c r="B434" t="s" s="2">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C434" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D434" s="2"/>
       <c r="E434" t="s" s="2">
@@ -50760,10 +50763,10 @@
         <v>858</v>
       </c>
       <c r="B435" t="s" s="2">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="C435" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D435" s="2"/>
       <c r="E435" t="s" s="2">
@@ -50865,10 +50868,10 @@
         <v>858</v>
       </c>
       <c r="B436" t="s" s="2">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C436" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D436" s="2"/>
       <c r="E436" t="s" s="2">
@@ -50972,14 +50975,14 @@
         <v>858</v>
       </c>
       <c r="B437" t="s" s="2">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C437" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D437" s="2"/>
       <c r="E437" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F437" s="2"/>
       <c r="G437" t="s" s="2">
@@ -51001,16 +51004,16 @@
         <v>354</v>
       </c>
       <c r="M437" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N437" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O437" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P437" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q437" t="s" s="2">
         <v>74</v>
@@ -51020,7 +51023,7 @@
         <v>74</v>
       </c>
       <c r="T437" t="s" s="2">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="U437" t="s" s="2">
         <v>74</v>
@@ -51038,7 +51041,7 @@
         <v>315</v>
       </c>
       <c r="Z437" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA437" t="s" s="2">
         <v>74</v>
@@ -51059,7 +51062,7 @@
         <v>74</v>
       </c>
       <c r="AG437" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH437" t="s" s="2">
         <v>82</v>
@@ -51079,10 +51082,10 @@
         <v>858</v>
       </c>
       <c r="B438" t="s" s="2">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="C438" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D438" s="2"/>
       <c r="E438" t="s" s="2">
@@ -51108,10 +51111,10 @@
         <v>354</v>
       </c>
       <c r="M438" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N438" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O438" s="2"/>
       <c r="P438" s="2"/>
@@ -51142,7 +51145,7 @@
       </c>
       <c r="Z438" s="2"/>
       <c r="AA438" t="s" s="2">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="AB438" t="s" s="2">
         <v>74</v>
@@ -51160,7 +51163,7 @@
         <v>74</v>
       </c>
       <c r="AG438" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH438" t="s" s="2">
         <v>82</v>
@@ -51180,16 +51183,16 @@
         <v>858</v>
       </c>
       <c r="B439" t="s" s="2">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="C439" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D439" t="s" s="2">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="E439" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F439" s="2"/>
       <c r="G439" t="s" s="2">
@@ -51211,14 +51214,14 @@
         <v>136</v>
       </c>
       <c r="M439" t="s" s="2">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="N439" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O439" s="2"/>
       <c r="P439" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q439" t="s" s="2">
         <v>74</v>
@@ -51267,7 +51270,7 @@
         <v>74</v>
       </c>
       <c r="AG439" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH439" t="s" s="2">
         <v>75</v>
@@ -51287,10 +51290,10 @@
         <v>858</v>
       </c>
       <c r="B440" t="s" s="2">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="C440" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D440" s="2"/>
       <c r="E440" t="s" s="2">
@@ -51390,10 +51393,10 @@
         <v>858</v>
       </c>
       <c r="B441" t="s" s="2">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="C441" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D441" s="2"/>
       <c r="E441" t="s" s="2">
@@ -51495,10 +51498,10 @@
         <v>858</v>
       </c>
       <c r="B442" t="s" s="2">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C442" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D442" s="2"/>
       <c r="E442" t="s" s="2">
@@ -51602,14 +51605,14 @@
         <v>858</v>
       </c>
       <c r="B443" t="s" s="2">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C443" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D443" s="2"/>
       <c r="E443" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F443" s="2"/>
       <c r="G443" t="s" s="2">
@@ -51631,16 +51634,16 @@
         <v>354</v>
       </c>
       <c r="M443" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N443" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O443" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P443" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q443" t="s" s="2">
         <v>74</v>
@@ -51650,7 +51653,7 @@
         <v>74</v>
       </c>
       <c r="T443" t="s" s="2">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="U443" t="s" s="2">
         <v>74</v>
@@ -51668,7 +51671,7 @@
         <v>315</v>
       </c>
       <c r="Z443" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA443" t="s" s="2">
         <v>74</v>
@@ -51689,7 +51692,7 @@
         <v>74</v>
       </c>
       <c r="AG443" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH443" t="s" s="2">
         <v>82</v>
@@ -51709,10 +51712,10 @@
         <v>858</v>
       </c>
       <c r="B444" t="s" s="2">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="C444" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D444" s="2"/>
       <c r="E444" t="s" s="2">
@@ -51738,10 +51741,10 @@
         <v>422</v>
       </c>
       <c r="M444" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N444" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O444" s="2"/>
       <c r="P444" s="2"/>
@@ -51792,7 +51795,7 @@
         <v>74</v>
       </c>
       <c r="AG444" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH444" t="s" s="2">
         <v>82</v>
@@ -51812,16 +51815,16 @@
         <v>858</v>
       </c>
       <c r="B445" t="s" s="2">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="C445" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D445" t="s" s="2">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="E445" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F445" s="2"/>
       <c r="G445" t="s" s="2">
@@ -51843,14 +51846,14 @@
         <v>136</v>
       </c>
       <c r="M445" t="s" s="2">
-        <v>1161</v>
+        <v>1162</v>
       </c>
       <c r="N445" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O445" s="2"/>
       <c r="P445" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q445" t="s" s="2">
         <v>74</v>
@@ -51899,7 +51902,7 @@
         <v>74</v>
       </c>
       <c r="AG445" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH445" t="s" s="2">
         <v>75</v>
@@ -51911,7 +51914,7 @@
         <v>94</v>
       </c>
       <c r="AK445" t="s" s="2">
-        <v>1162</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="446">
@@ -51919,10 +51922,10 @@
         <v>858</v>
       </c>
       <c r="B446" t="s" s="2">
-        <v>1163</v>
+        <v>1164</v>
       </c>
       <c r="C446" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D446" s="2"/>
       <c r="E446" t="s" s="2">
@@ -52022,10 +52025,10 @@
         <v>858</v>
       </c>
       <c r="B447" t="s" s="2">
-        <v>1164</v>
+        <v>1165</v>
       </c>
       <c r="C447" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D447" s="2"/>
       <c r="E447" t="s" s="2">
@@ -52127,10 +52130,10 @@
         <v>858</v>
       </c>
       <c r="B448" t="s" s="2">
-        <v>1165</v>
+        <v>1166</v>
       </c>
       <c r="C448" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D448" s="2"/>
       <c r="E448" t="s" s="2">
@@ -52234,14 +52237,14 @@
         <v>858</v>
       </c>
       <c r="B449" t="s" s="2">
-        <v>1166</v>
+        <v>1167</v>
       </c>
       <c r="C449" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D449" s="2"/>
       <c r="E449" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F449" s="2"/>
       <c r="G449" t="s" s="2">
@@ -52263,16 +52266,16 @@
         <v>354</v>
       </c>
       <c r="M449" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N449" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O449" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P449" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q449" t="s" s="2">
         <v>74</v>
@@ -52282,7 +52285,7 @@
         <v>74</v>
       </c>
       <c r="T449" t="s" s="2">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="U449" t="s" s="2">
         <v>74</v>
@@ -52300,7 +52303,7 @@
         <v>315</v>
       </c>
       <c r="Z449" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA449" t="s" s="2">
         <v>74</v>
@@ -52321,7 +52324,7 @@
         <v>74</v>
       </c>
       <c r="AG449" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH449" t="s" s="2">
         <v>82</v>
@@ -52341,10 +52344,10 @@
         <v>858</v>
       </c>
       <c r="B450" t="s" s="2">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="C450" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D450" s="2"/>
       <c r="E450" t="s" s="2">
@@ -52370,10 +52373,10 @@
         <v>354</v>
       </c>
       <c r="M450" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N450" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O450" s="2"/>
       <c r="P450" s="2"/>
@@ -52404,7 +52407,7 @@
       </c>
       <c r="Z450" s="2"/>
       <c r="AA450" t="s" s="2">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="AB450" t="s" s="2">
         <v>74</v>
@@ -52422,7 +52425,7 @@
         <v>74</v>
       </c>
       <c r="AG450" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH450" t="s" s="2">
         <v>82</v>
@@ -52442,10 +52445,10 @@
         <v>858</v>
       </c>
       <c r="B451" t="s" s="2">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="C451" t="s" s="2">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D451" s="2"/>
       <c r="E451" t="s" s="2">
@@ -52545,10 +52548,10 @@
         <v>858</v>
       </c>
       <c r="B452" t="s" s="2">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="C452" t="s" s="2">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="D452" s="2"/>
       <c r="E452" t="s" s="2">
@@ -52650,10 +52653,10 @@
         <v>858</v>
       </c>
       <c r="B453" t="s" s="2">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="C453" t="s" s="2">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="D453" s="2"/>
       <c r="E453" t="s" s="2">
@@ -52757,10 +52760,10 @@
         <v>858</v>
       </c>
       <c r="B454" t="s" s="2">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="C454" t="s" s="2">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D454" s="2"/>
       <c r="E454" t="s" s="2">
@@ -52864,16 +52867,16 @@
         <v>858</v>
       </c>
       <c r="B455" t="s" s="2">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="C455" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D455" t="s" s="2">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="E455" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F455" s="2"/>
       <c r="G455" t="s" s="2">
@@ -52895,14 +52898,14 @@
         <v>136</v>
       </c>
       <c r="M455" t="s" s="2">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="N455" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O455" s="2"/>
       <c r="P455" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q455" t="s" s="2">
         <v>74</v>
@@ -52951,7 +52954,7 @@
         <v>74</v>
       </c>
       <c r="AG455" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH455" t="s" s="2">
         <v>75</v>
@@ -52971,10 +52974,10 @@
         <v>858</v>
       </c>
       <c r="B456" t="s" s="2">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="C456" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D456" s="2"/>
       <c r="E456" t="s" s="2">
@@ -53074,10 +53077,10 @@
         <v>858</v>
       </c>
       <c r="B457" t="s" s="2">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="C457" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D457" s="2"/>
       <c r="E457" t="s" s="2">
@@ -53179,10 +53182,10 @@
         <v>858</v>
       </c>
       <c r="B458" t="s" s="2">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C458" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D458" s="2"/>
       <c r="E458" t="s" s="2">
@@ -53286,14 +53289,14 @@
         <v>858</v>
       </c>
       <c r="B459" t="s" s="2">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="C459" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D459" s="2"/>
       <c r="E459" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F459" s="2"/>
       <c r="G459" t="s" s="2">
@@ -53315,16 +53318,16 @@
         <v>354</v>
       </c>
       <c r="M459" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N459" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O459" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P459" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q459" t="s" s="2">
         <v>74</v>
@@ -53334,7 +53337,7 @@
         <v>74</v>
       </c>
       <c r="T459" t="s" s="2">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="U459" t="s" s="2">
         <v>74</v>
@@ -53352,7 +53355,7 @@
         <v>315</v>
       </c>
       <c r="Z459" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA459" t="s" s="2">
         <v>74</v>
@@ -53373,7 +53376,7 @@
         <v>74</v>
       </c>
       <c r="AG459" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH459" t="s" s="2">
         <v>82</v>
@@ -53393,10 +53396,10 @@
         <v>858</v>
       </c>
       <c r="B460" t="s" s="2">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="C460" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D460" s="2"/>
       <c r="E460" t="s" s="2">
@@ -53422,10 +53425,10 @@
         <v>354</v>
       </c>
       <c r="M460" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N460" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O460" s="2"/>
       <c r="P460" s="2"/>
@@ -53456,7 +53459,7 @@
       </c>
       <c r="Z460" s="2"/>
       <c r="AA460" t="s" s="2">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="AB460" t="s" s="2">
         <v>74</v>
@@ -53474,7 +53477,7 @@
         <v>74</v>
       </c>
       <c r="AG460" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH460" t="s" s="2">
         <v>82</v>
@@ -53494,16 +53497,16 @@
         <v>858</v>
       </c>
       <c r="B461" t="s" s="2">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="C461" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D461" t="s" s="2">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="E461" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F461" s="2"/>
       <c r="G461" t="s" s="2">
@@ -53525,14 +53528,14 @@
         <v>136</v>
       </c>
       <c r="M461" t="s" s="2">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="N461" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O461" s="2"/>
       <c r="P461" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q461" t="s" s="2">
         <v>74</v>
@@ -53581,7 +53584,7 @@
         <v>74</v>
       </c>
       <c r="AG461" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH461" t="s" s="2">
         <v>75</v>
@@ -53601,10 +53604,10 @@
         <v>858</v>
       </c>
       <c r="B462" t="s" s="2">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="C462" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D462" s="2"/>
       <c r="E462" t="s" s="2">
@@ -53704,10 +53707,10 @@
         <v>858</v>
       </c>
       <c r="B463" t="s" s="2">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="C463" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D463" s="2"/>
       <c r="E463" t="s" s="2">
@@ -53809,10 +53812,10 @@
         <v>858</v>
       </c>
       <c r="B464" t="s" s="2">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="C464" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D464" s="2"/>
       <c r="E464" t="s" s="2">
@@ -53916,14 +53919,14 @@
         <v>858</v>
       </c>
       <c r="B465" t="s" s="2">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="C465" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D465" s="2"/>
       <c r="E465" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F465" s="2"/>
       <c r="G465" t="s" s="2">
@@ -53945,16 +53948,16 @@
         <v>354</v>
       </c>
       <c r="M465" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N465" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O465" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P465" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q465" t="s" s="2">
         <v>74</v>
@@ -53964,7 +53967,7 @@
         <v>74</v>
       </c>
       <c r="T465" t="s" s="2">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="U465" t="s" s="2">
         <v>74</v>
@@ -53982,7 +53985,7 @@
         <v>315</v>
       </c>
       <c r="Z465" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA465" t="s" s="2">
         <v>74</v>
@@ -54003,7 +54006,7 @@
         <v>74</v>
       </c>
       <c r="AG465" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH465" t="s" s="2">
         <v>82</v>
@@ -54023,10 +54026,10 @@
         <v>858</v>
       </c>
       <c r="B466" t="s" s="2">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="C466" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D466" s="2"/>
       <c r="E466" t="s" s="2">
@@ -54049,13 +54052,13 @@
         <v>74</v>
       </c>
       <c r="L466" t="s" s="2">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="M466" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N466" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O466" s="2"/>
       <c r="P466" s="2"/>
@@ -54106,7 +54109,7 @@
         <v>74</v>
       </c>
       <c r="AG466" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH466" t="s" s="2">
         <v>82</v>
@@ -54126,16 +54129,16 @@
         <v>858</v>
       </c>
       <c r="B467" t="s" s="2">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="C467" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D467" t="s" s="2">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="E467" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F467" s="2"/>
       <c r="G467" t="s" s="2">
@@ -54157,14 +54160,14 @@
         <v>136</v>
       </c>
       <c r="M467" t="s" s="2">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="N467" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O467" s="2"/>
       <c r="P467" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q467" t="s" s="2">
         <v>74</v>
@@ -54213,7 +54216,7 @@
         <v>74</v>
       </c>
       <c r="AG467" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH467" t="s" s="2">
         <v>75</v>
@@ -54233,10 +54236,10 @@
         <v>858</v>
       </c>
       <c r="B468" t="s" s="2">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="C468" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D468" s="2"/>
       <c r="E468" t="s" s="2">
@@ -54336,10 +54339,10 @@
         <v>858</v>
       </c>
       <c r="B469" t="s" s="2">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="C469" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D469" s="2"/>
       <c r="E469" t="s" s="2">
@@ -54441,10 +54444,10 @@
         <v>858</v>
       </c>
       <c r="B470" t="s" s="2">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="C470" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D470" s="2"/>
       <c r="E470" t="s" s="2">
@@ -54548,14 +54551,14 @@
         <v>858</v>
       </c>
       <c r="B471" t="s" s="2">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="C471" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D471" s="2"/>
       <c r="E471" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F471" s="2"/>
       <c r="G471" t="s" s="2">
@@ -54577,16 +54580,16 @@
         <v>354</v>
       </c>
       <c r="M471" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N471" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O471" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P471" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q471" t="s" s="2">
         <v>74</v>
@@ -54596,7 +54599,7 @@
         <v>74</v>
       </c>
       <c r="T471" t="s" s="2">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="U471" t="s" s="2">
         <v>74</v>
@@ -54614,7 +54617,7 @@
         <v>315</v>
       </c>
       <c r="Z471" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA471" t="s" s="2">
         <v>74</v>
@@ -54635,7 +54638,7 @@
         <v>74</v>
       </c>
       <c r="AG471" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH471" t="s" s="2">
         <v>82</v>
@@ -54655,10 +54658,10 @@
         <v>858</v>
       </c>
       <c r="B472" t="s" s="2">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="C472" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D472" s="2"/>
       <c r="E472" t="s" s="2">
@@ -54684,10 +54687,10 @@
         <v>354</v>
       </c>
       <c r="M472" t="s" s="2">
-        <v>1206</v>
+        <v>1207</v>
       </c>
       <c r="N472" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O472" s="2"/>
       <c r="P472" s="2"/>
@@ -54718,7 +54721,7 @@
       </c>
       <c r="Z472" s="2"/>
       <c r="AA472" t="s" s="2">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="AB472" t="s" s="2">
         <v>74</v>
@@ -54736,7 +54739,7 @@
         <v>74</v>
       </c>
       <c r="AG472" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH472" t="s" s="2">
         <v>82</v>
@@ -54756,16 +54759,16 @@
         <v>858</v>
       </c>
       <c r="B473" t="s" s="2">
-        <v>1208</v>
+        <v>1209</v>
       </c>
       <c r="C473" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D473" t="s" s="2">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="E473" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F473" s="2"/>
       <c r="G473" t="s" s="2">
@@ -54787,14 +54790,14 @@
         <v>136</v>
       </c>
       <c r="M473" t="s" s="2">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="N473" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O473" s="2"/>
       <c r="P473" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q473" t="s" s="2">
         <v>74</v>
@@ -54843,7 +54846,7 @@
         <v>74</v>
       </c>
       <c r="AG473" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH473" t="s" s="2">
         <v>75</v>
@@ -54863,10 +54866,10 @@
         <v>858</v>
       </c>
       <c r="B474" t="s" s="2">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="C474" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D474" s="2"/>
       <c r="E474" t="s" s="2">
@@ -54966,10 +54969,10 @@
         <v>858</v>
       </c>
       <c r="B475" t="s" s="2">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="C475" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D475" s="2"/>
       <c r="E475" t="s" s="2">
@@ -55071,10 +55074,10 @@
         <v>858</v>
       </c>
       <c r="B476" t="s" s="2">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="C476" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D476" s="2"/>
       <c r="E476" t="s" s="2">
@@ -55178,14 +55181,14 @@
         <v>858</v>
       </c>
       <c r="B477" t="s" s="2">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="C477" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D477" s="2"/>
       <c r="E477" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F477" s="2"/>
       <c r="G477" t="s" s="2">
@@ -55207,16 +55210,16 @@
         <v>354</v>
       </c>
       <c r="M477" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N477" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O477" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P477" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q477" t="s" s="2">
         <v>74</v>
@@ -55226,7 +55229,7 @@
         <v>74</v>
       </c>
       <c r="T477" t="s" s="2">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="U477" t="s" s="2">
         <v>74</v>
@@ -55244,7 +55247,7 @@
         <v>315</v>
       </c>
       <c r="Z477" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA477" t="s" s="2">
         <v>74</v>
@@ -55265,7 +55268,7 @@
         <v>74</v>
       </c>
       <c r="AG477" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH477" t="s" s="2">
         <v>82</v>
@@ -55285,10 +55288,10 @@
         <v>858</v>
       </c>
       <c r="B478" t="s" s="2">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="C478" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D478" s="2"/>
       <c r="E478" t="s" s="2">
@@ -55314,10 +55317,10 @@
         <v>354</v>
       </c>
       <c r="M478" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N478" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O478" s="2"/>
       <c r="P478" s="2"/>
@@ -55348,7 +55351,7 @@
       </c>
       <c r="Z478" s="2"/>
       <c r="AA478" t="s" s="2">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="AB478" t="s" s="2">
         <v>74</v>
@@ -55366,7 +55369,7 @@
         <v>74</v>
       </c>
       <c r="AG478" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH478" t="s" s="2">
         <v>82</v>
@@ -55386,16 +55389,16 @@
         <v>858</v>
       </c>
       <c r="B479" t="s" s="2">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="C479" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D479" t="s" s="2">
         <v>612</v>
       </c>
       <c r="E479" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F479" s="2"/>
       <c r="G479" t="s" s="2">
@@ -55417,14 +55420,14 @@
         <v>136</v>
       </c>
       <c r="M479" t="s" s="2">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="N479" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O479" s="2"/>
       <c r="P479" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q479" t="s" s="2">
         <v>74</v>
@@ -55473,7 +55476,7 @@
         <v>74</v>
       </c>
       <c r="AG479" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH479" t="s" s="2">
         <v>75</v>
@@ -55493,10 +55496,10 @@
         <v>858</v>
       </c>
       <c r="B480" t="s" s="2">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="C480" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D480" s="2"/>
       <c r="E480" t="s" s="2">
@@ -55596,10 +55599,10 @@
         <v>858</v>
       </c>
       <c r="B481" t="s" s="2">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="C481" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D481" s="2"/>
       <c r="E481" t="s" s="2">
@@ -55701,10 +55704,10 @@
         <v>858</v>
       </c>
       <c r="B482" t="s" s="2">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="C482" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D482" s="2"/>
       <c r="E482" t="s" s="2">
@@ -55808,14 +55811,14 @@
         <v>858</v>
       </c>
       <c r="B483" t="s" s="2">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="C483" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D483" s="2"/>
       <c r="E483" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F483" s="2"/>
       <c r="G483" t="s" s="2">
@@ -55837,16 +55840,16 @@
         <v>354</v>
       </c>
       <c r="M483" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N483" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O483" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P483" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q483" t="s" s="2">
         <v>74</v>
@@ -55856,7 +55859,7 @@
         <v>74</v>
       </c>
       <c r="T483" t="s" s="2">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="U483" t="s" s="2">
         <v>74</v>
@@ -55874,7 +55877,7 @@
         <v>315</v>
       </c>
       <c r="Z483" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA483" t="s" s="2">
         <v>74</v>
@@ -55895,7 +55898,7 @@
         <v>74</v>
       </c>
       <c r="AG483" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH483" t="s" s="2">
         <v>82</v>
@@ -55915,10 +55918,10 @@
         <v>858</v>
       </c>
       <c r="B484" t="s" s="2">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="C484" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D484" s="2"/>
       <c r="E484" t="s" s="2">
@@ -55944,10 +55947,10 @@
         <v>112</v>
       </c>
       <c r="M484" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N484" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O484" s="2"/>
       <c r="P484" s="2"/>
@@ -55998,7 +56001,7 @@
         <v>74</v>
       </c>
       <c r="AG484" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH484" t="s" s="2">
         <v>82</v>
@@ -56018,16 +56021,16 @@
         <v>858</v>
       </c>
       <c r="B485" t="s" s="2">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="C485" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D485" t="s" s="2">
         <v>633</v>
       </c>
       <c r="E485" t="s" s="2">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="F485" s="2"/>
       <c r="G485" t="s" s="2">
@@ -56049,14 +56052,14 @@
         <v>136</v>
       </c>
       <c r="M485" t="s" s="2">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="N485" t="s" s="2">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="O485" s="2"/>
       <c r="P485" t="s" s="2">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="Q485" t="s" s="2">
         <v>74</v>
@@ -56105,7 +56108,7 @@
         <v>74</v>
       </c>
       <c r="AG485" t="s" s="2">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="AH485" t="s" s="2">
         <v>75</v>
@@ -56125,10 +56128,10 @@
         <v>858</v>
       </c>
       <c r="B486" t="s" s="2">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="C486" t="s" s="2">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="D486" s="2"/>
       <c r="E486" t="s" s="2">
@@ -56228,10 +56231,10 @@
         <v>858</v>
       </c>
       <c r="B487" t="s" s="2">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="C487" t="s" s="2">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D487" s="2"/>
       <c r="E487" t="s" s="2">
@@ -56333,10 +56336,10 @@
         <v>858</v>
       </c>
       <c r="B488" t="s" s="2">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="C488" t="s" s="2">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D488" s="2"/>
       <c r="E488" t="s" s="2">
@@ -56440,14 +56443,14 @@
         <v>858</v>
       </c>
       <c r="B489" t="s" s="2">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="C489" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D489" s="2"/>
       <c r="E489" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F489" s="2"/>
       <c r="G489" t="s" s="2">
@@ -56469,16 +56472,16 @@
         <v>354</v>
       </c>
       <c r="M489" t="s" s="2">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N489" t="s" s="2">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="O489" t="s" s="2">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="P489" t="s" s="2">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="Q489" t="s" s="2">
         <v>74</v>
@@ -56488,7 +56491,7 @@
         <v>74</v>
       </c>
       <c r="T489" t="s" s="2">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="U489" t="s" s="2">
         <v>74</v>
@@ -56506,7 +56509,7 @@
         <v>315</v>
       </c>
       <c r="Z489" t="s" s="2">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AA489" t="s" s="2">
         <v>74</v>
@@ -56527,7 +56530,7 @@
         <v>74</v>
       </c>
       <c r="AG489" t="s" s="2">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH489" t="s" s="2">
         <v>82</v>
@@ -56547,10 +56550,10 @@
         <v>858</v>
       </c>
       <c r="B490" t="s" s="2">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="C490" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="D490" s="2"/>
       <c r="E490" t="s" s="2">
@@ -56576,10 +56579,10 @@
         <v>112</v>
       </c>
       <c r="M490" t="s" s="2">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="N490" t="s" s="2">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="O490" s="2"/>
       <c r="P490" s="2"/>
@@ -56630,7 +56633,7 @@
         <v>74</v>
       </c>
       <c r="AG490" t="s" s="2">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="AH490" t="s" s="2">
         <v>82</v>
@@ -56650,10 +56653,10 @@
         <v>858</v>
       </c>
       <c r="B491" t="s" s="2">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="C491" t="s" s="2">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D491" s="2"/>
       <c r="E491" t="s" s="2">
@@ -56679,14 +56682,14 @@
         <v>136</v>
       </c>
       <c r="M491" t="s" s="2">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="N491" t="s" s="2">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="O491" s="2"/>
       <c r="P491" t="s" s="2">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="Q491" t="s" s="2">
         <v>74</v>
@@ -56735,7 +56738,7 @@
         <v>74</v>
       </c>
       <c r="AG491" t="s" s="2">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="AH491" t="s" s="2">
         <v>75</v>
@@ -56755,10 +56758,10 @@
         <v>858</v>
       </c>
       <c r="B492" t="s" s="2">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="C492" t="s" s="2">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="D492" s="2"/>
       <c r="E492" t="s" s="2">
@@ -56858,10 +56861,10 @@
         <v>858</v>
       </c>
       <c r="B493" t="s" s="2">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="C493" t="s" s="2">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="D493" s="2"/>
       <c r="E493" t="s" s="2">
@@ -56963,10 +56966,10 @@
         <v>858</v>
       </c>
       <c r="B494" t="s" s="2">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="C494" t="s" s="2">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="D494" s="2"/>
       <c r="E494" t="s" s="2">
@@ -57070,14 +57073,14 @@
         <v>858</v>
       </c>
       <c r="B495" t="s" s="2">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="C495" t="s" s="2">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="D495" s="2"/>
       <c r="E495" t="s" s="2">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F495" s="2"/>
       <c r="G495" t="s" s="2">
@@ -57099,16 +57102,16 @@
         <v>354</v>
       </c>
       <c r="M495" t="s" s="2">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="N495" t="s" s="2">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="O495" t="s" s="2">
         <v>357</v>
       </c>
       <c r="P495" t="s" s="2">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="Q495" t="s" s="2">
         <v>74</v>
@@ -57136,7 +57139,7 @@
         <v>315</v>
       </c>
       <c r="Z495" t="s" s="2">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="AA495" t="s" s="2">
         <v>74</v>
@@ -57157,7 +57160,7 @@
         <v>74</v>
       </c>
       <c r="AG495" t="s" s="2">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="AH495" t="s" s="2">
         <v>82</v>
@@ -57177,10 +57180,10 @@
         <v>858</v>
       </c>
       <c r="B496" t="s" s="2">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="C496" t="s" s="2">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="D496" s="2"/>
       <c r="E496" t="s" s="2">
@@ -57203,17 +57206,17 @@
         <v>74</v>
       </c>
       <c r="L496" t="s" s="2">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="M496" t="s" s="2">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="N496" t="s" s="2">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="O496" s="2"/>
       <c r="P496" t="s" s="2">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="Q496" t="s" s="2">
         <v>74</v>
@@ -57262,7 +57265,7 @@
         <v>74</v>
       </c>
       <c r="AG496" t="s" s="2">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="AH496" t="s" s="2">
         <v>82</v>

</xml_diff>